<commit_message>
More bug fixes. Mainly getting the spelling of the fish composites correct.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/retentionLookup.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/retentionLookup.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/nutrientDetails/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF37310C-273C-3148-8235-C2CE702CAE83}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="2380" windowWidth="24200" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="4180" yWindow="2380" windowWidth="24200" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$52</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -296,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -425,14 +426,17 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 5" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -700,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1349,7 +1353,7 @@
         <v>62</v>
       </c>
       <c r="B60" s="17">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>81</v>
@@ -1360,7 +1364,7 @@
         <v>63</v>
       </c>
       <c r="B61" s="17">
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>81</v>
@@ -1371,14 +1375,14 @@
         <v>64</v>
       </c>
       <c r="B62" s="17">
-        <v>2404</v>
+        <v>2401</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B52"/>
+  <autoFilter ref="A1:B52" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="A2:C53">
     <sortCondition ref="B2:B53"/>
   </sortState>

</xml_diff>